<commit_message>
added node and asp.net core project skeletons. updated procedures and data model
</commit_message>
<xml_diff>
--- a/SM_testData.xlsx
+++ b/SM_testData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coneill/Documents/repos/ScienceMine/Database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coneill/rfs/csdept17/projects/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFF7BF1-7AB3-0A48-B95A-5250A9216760}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3417D4-9202-3245-A4BE-1D4BB1511DB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1490,11 +1490,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1908,9 +1910,9 @@
   </sheetPr>
   <dimension ref="A1:O189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K191" sqref="K191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1993,8 +1995,8 @@
         <v>2018-09-05</v>
       </c>
       <c r="O2" t="str">
-        <f>_xlfn.CONCAT("call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '", L2, "', '", M2, "'); call addPrimaryMember(@membershipId,'", B2, "', '", A2, "', 25, null, 'male', null, '", J2, "', '", H2, "', null, null,'", D2, "', '", C2, "', 'MT');")</f>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-09-05', '2018-09-05'); call addPrimaryMember(@membershipId,'Theron', 'Wilson', 25, null, 'male', null, '', '', null, null,'Butte', '59701', 'MT');</v>
+        <f>_xlfn.CONCAT("call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '", L2, "', '", M2, "'); call addMember(@membershipId,'", B2, "', '", A2, "', 25, null, 'male', null, '", J2, "', '", H2, "', null, null,'", D2, "', '", C2, "', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);")</f>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-09-05', '2018-09-05'); call addMember(@membershipId,'Theron', 'Wilson', 25, null, 'male', null, '', '', null, null,'Butte', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2028,8 +2030,8 @@
         <v>2016-02-06</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O66" si="2">_xlfn.CONCAT("call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '", L3, "', '", M3, "'); call addPrimaryMember(@membershipId,'", B3, "', '", A3, "', 25, null, 'male', null, '", J3, "', '", H3, "', null, null,'", D3, "', '", C3, "', 'MT');")</f>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-06', '2016-02-06'); call addPrimaryMember(@membershipId,'Dawn', 'Wilcox', 25, null, 'male', null, '', 'dgordon7229@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <f t="shared" ref="O3:O66" si="2">_xlfn.CONCAT("call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '", L3, "', '", M3, "'); call addMember(@membershipId,'", B3, "', '", A3, "', 25, null, 'male', null, '", J3, "', '", H3, "', null, null,'", D3, "', '", C3, "', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);")</f>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-06', '2016-02-06'); call addMember(@membershipId,'Dawn', 'Wilcox', 25, null, 'male', null, '', 'dgordon7229@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2064,7 +2066,7 @@
       </c>
       <c r="O4" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-18', '2016-04-18'); call addPrimaryMember(@membershipId,'Jordan', 'Stevens', 25, null, 'male', null, '4066985698', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-18', '2016-04-18'); call addMember(@membershipId,'Jordan', 'Stevens', 25, null, 'male', null, '4066985698', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2096,7 +2098,7 @@
       </c>
       <c r="O5" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addPrimaryMember(@membershipId,'', 'Andersen', 25, null, 'male', null, '', 'phippsallijo@juno.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addMember(@membershipId,'', 'Andersen', 25, null, 'male', null, '', 'phippsallijo@juno.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2131,7 +2133,7 @@
       </c>
       <c r="O6" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addPrimaryMember(@membershipId,'Susan', 'Schrader', 25, null, 'male', null, '', 'sschrader@mtech.edu', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addMember(@membershipId,'Susan', 'Schrader', 25, null, 'male', null, '', 'sschrader@mtech.edu', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2161,7 +2163,7 @@
       </c>
       <c r="O7" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addPrimaryMember(@membershipId,'', 'O'Donnell', 25, null, 'male', null, '', 'serenityodonnell@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addMember(@membershipId,'', 'O'Donnell', 25, null, 'male', null, '', 'serenityodonnell@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2194,7 +2196,7 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addPrimaryMember(@membershipId,'Jamie', 'Offutt', 25, null, 'male', null, '', 'phobia-@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addMember(@membershipId,'Jamie', 'Offutt', 25, null, 'male', null, '', 'phobia-@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2227,7 +2229,7 @@
       </c>
       <c r="O9" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addPrimaryMember(@membershipId,'Cheryl', 'Madison', 25, null, 'male', null, '', 'euhedral@msn.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addMember(@membershipId,'Cheryl', 'Madison', 25, null, 'male', null, '', 'euhedral@msn.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2256,7 +2258,7 @@
       </c>
       <c r="O10" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addPrimaryMember(@membershipId,'Vik', 'Kujawa', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addMember(@membershipId,'Vik', 'Kujawa', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2292,7 +2294,7 @@
       </c>
       <c r="O11" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-04', '2016-04-04'); call addPrimaryMember(@membershipId,'Kels', 'Brodie', 25, null, 'male', null, '', 'bchoops1@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-04', '2016-04-04'); call addMember(@membershipId,'Kels', 'Brodie', 25, null, 'male', null, '', 'bchoops1@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2327,7 +2329,7 @@
       </c>
       <c r="O12" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-21', '2016-03-21'); call addPrimaryMember(@membershipId,'Bill', 'Burger', 25, null, 'male', null, '', 'burger_bill@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-21', '2016-03-21'); call addMember(@membershipId,'Bill', 'Burger', 25, null, 'male', null, '', 'burger_bill@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2362,7 +2364,7 @@
       </c>
       <c r="O13" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-28', '2016-03-28'); call addPrimaryMember(@membershipId,'Mack', 'Gollinger', 25, null, 'male', null, '', 'mpgollinger@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-28', '2016-03-28'); call addMember(@membershipId,'Mack', 'Gollinger', 25, null, 'male', null, '', 'mpgollinger@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2397,7 +2399,7 @@
       </c>
       <c r="O14" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-21', '2016-03-21'); call addPrimaryMember(@membershipId,'Michelle', 'Wold', 25, null, 'male', null, '7828921', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-21', '2016-03-21'); call addMember(@membershipId,'Michelle', 'Wold', 25, null, 'male', null, '7828921', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2435,7 +2437,7 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-04', '2016-04-04'); call addPrimaryMember(@membershipId,'Dianna', 'Porter ', 25, null, 'male', null, '', 'porterdianna@hotmail.com', null, null,'', '59703', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-04', '2016-04-04'); call addMember(@membershipId,'Dianna', 'Porter ', 25, null, 'male', null, '', 'porterdianna@hotmail.com', null, null,'', '59703', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2472,7 +2474,7 @@
       </c>
       <c r="O16" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-28', '2016-03-28'); call addPrimaryMember(@membershipId,'Kim', 'Mannix', 25, null, 'male', null, '7234191', 'kqbrown@msn.com  ', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-28', '2016-03-28'); call addMember(@membershipId,'Kim', 'Mannix', 25, null, 'male', null, '7234191', 'kqbrown@msn.com  ', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2509,7 +2511,7 @@
       </c>
       <c r="O17" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2002-04-18', '2003-04-18'); call addPrimaryMember(@membershipId,'Michelle', 'Zarate', 25, null, 'male', null, '4064984627', 'nieinazakat@live.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2002-04-18', '2003-04-18'); call addMember(@membershipId,'Michelle', 'Zarate', 25, null, 'male', null, '4064984627', 'nieinazakat@live.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2547,7 +2549,7 @@
       </c>
       <c r="O18" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-14', '2016-03-14'); call addPrimaryMember(@membershipId,'Kevin', 'Pfeifer', 25, null, 'male', null, '', 'kwpfeifer@gmail.com', null, null,'Anaconda', '59711', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-14', '2016-03-14'); call addMember(@membershipId,'Kevin', 'Pfeifer', 25, null, 'male', null, '', 'kwpfeifer@gmail.com', null, null,'Anaconda', '59711', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2583,7 +2585,7 @@
       </c>
       <c r="O19" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-04', '2016-04-04'); call addPrimaryMember(@membershipId,'Steve', 'Hess', 25, null, 'male', null, '', 'shess@bsb.mt.gov', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-04', '2016-04-04'); call addMember(@membershipId,'Steve', 'Hess', 25, null, 'male', null, '', 'shess@bsb.mt.gov', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2615,7 +2617,7 @@
       </c>
       <c r="O20" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'', 'Vincent', 25, null, 'male', null, '', 'ajkvincent@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'', 'Vincent', 25, null, 'male', null, '', 'ajkvincent@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2641,7 +2643,7 @@
       </c>
       <c r="O21" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'', 'Watson', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'', 'Watson', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2676,7 +2678,7 @@
       </c>
       <c r="O22" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'Suzanne', 'Stefanac', 25, null, 'male', null, '', 'suzanne.stefanac@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'Suzanne', 'Stefanac', 25, null, 'male', null, '', 'suzanne.stefanac@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2708,7 +2710,7 @@
       </c>
       <c r="O23" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'Marvin', 'Speece', 25, null, 'male', null, '', 'mspeece@mtech.edu', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'Marvin', 'Speece', 25, null, 'male', null, '', 'mspeece@mtech.edu', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2740,7 +2742,7 @@
       </c>
       <c r="O24" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'', 'Shadow', 25, null, 'male', null, '', 'sonjashadow@hmail.com', null, null,'Anaconda', '59711', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'', 'Shadow', 25, null, 'male', null, '', 'sonjashadow@hmail.com', null, null,'Anaconda', '59711', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2769,7 +2771,7 @@
       </c>
       <c r="O25" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'', 'Sawyer', 25, null, 'male', null, '', '', null, null,'Anaconda', '59711', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'', 'Sawyer', 25, null, 'male', null, '', '', null, null,'Anaconda', '59711', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2807,7 +2809,7 @@
       </c>
       <c r="O26" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'Chris/Lyndsay', 'Richards', 25, null, 'male', null, '', 'lapulrer01@gmail.com', null, null,'Three Forks', '59752', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'Chris/Lyndsay', 'Richards', 25, null, 'male', null, '', 'lapulrer01@gmail.com', null, null,'Three Forks', '59752', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2839,7 +2841,7 @@
       </c>
       <c r="O27" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addPrimaryMember(@membershipId,'Joe', 'Petroni-Jodel', 25, null, 'male', null, '', '3019 Atherton Ln', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addMember(@membershipId,'Joe', 'Petroni-Jodel', 25, null, 'male', null, '', '3019 Atherton Ln', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2874,7 +2876,7 @@
       </c>
       <c r="O28" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'Chris ', 'Lu', 25, null, 'male', null, '', 'jdt2009@live.com', null, null,'Billings', '59041', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'Chris ', 'Lu', 25, null, 'male', null, '', 'jdt2009@live.com', null, null,'Billings', '59041', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2906,7 +2908,7 @@
       </c>
       <c r="O29" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-01-07', '2016-01-07'); call addPrimaryMember(@membershipId,'Dave', 'Johns', 25, null, 'male', null, '', 'djohns523@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-01-07', '2016-01-07'); call addMember(@membershipId,'Dave', 'Johns', 25, null, 'male', null, '', 'djohns523@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2938,7 +2940,7 @@
       </c>
       <c r="O30" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-06', '2016-02-06'); call addPrimaryMember(@membershipId,'Robert/Tabatha', 'Hyatt', 25, null, 'male', null, '', 'tabathae@outlook.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-06', '2016-02-06'); call addMember(@membershipId,'Robert/Tabatha', 'Hyatt', 25, null, 'male', null, '', 'tabathae@outlook.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2976,7 +2978,7 @@
       </c>
       <c r="O31" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'Shaun', 'Hoolahan', 25, null, 'male', null, '', 'shoolahan@hotmail.com', null, null,'Anaconda', '59711', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'Shaun', 'Hoolahan', 25, null, 'male', null, '', 'shoolahan@hotmail.com', null, null,'Anaconda', '59711', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3008,7 +3010,7 @@
       </c>
       <c r="O32" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-06', '2016-02-06'); call addPrimaryMember(@membershipId,'Lisa', 'Graham', 25, null, 'male', null, '', 'lisagh20@gmail.com', null, null,'', '59759', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-06', '2016-02-06'); call addMember(@membershipId,'Lisa', 'Graham', 25, null, 'male', null, '', 'lisagh20@gmail.com', null, null,'', '59759', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3043,7 +3045,7 @@
       </c>
       <c r="O33" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'Mike', 'Flanick', 25, null, 'male', null, '', 'mflanick@gmail.com', null, null,'Ramsay', '59748', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'Mike', 'Flanick', 25, null, 'male', null, '', 'mflanick@gmail.com', null, null,'Ramsay', '59748', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3078,7 +3080,7 @@
       </c>
       <c r="O34" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'Erin', 'Angove', 25, null, 'male', null, '', 'becta@q.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'Erin', 'Angove', 25, null, 'male', null, '', 'becta@q.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3107,7 +3109,7 @@
       </c>
       <c r="O35" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'Gene', 'Ashby', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'Gene', 'Ashby', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3133,7 +3135,7 @@
       </c>
       <c r="O36" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'', 'Aware on Ottawa', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'', 'Aware on Ottawa', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3168,7 +3170,7 @@
       </c>
       <c r="O37" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addPrimaryMember(@membershipId,'Janet/Stephen', 'Coe', 25, null, 'male', null, '', 'janetmcoe@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-07', '2016-02-07'); call addMember(@membershipId,'Janet/Stephen', 'Coe', 25, null, 'male', null, '', 'janetmcoe@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3206,7 +3208,7 @@
       </c>
       <c r="O38" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addPrimaryMember(@membershipId,'Patrick', 'Andre ', 25, null, 'male', null, '', 'salutpandre@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addMember(@membershipId,'Patrick', 'Andre ', 25, null, 'male', null, '', 'salutpandre@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3244,7 +3246,7 @@
       </c>
       <c r="O39" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addPrimaryMember(@membershipId,'Wanda', 'Haller', 25, null, 'male', null, '', 'wandakp@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addMember(@membershipId,'Wanda', 'Haller', 25, null, 'male', null, '', 'wandakp@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3279,7 +3281,7 @@
       </c>
       <c r="O40" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addPrimaryMember(@membershipId,'Mickal', 'McCarthy', 25, null, 'male', null, '', 'mrmccarthy58@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addMember(@membershipId,'Mickal', 'McCarthy', 25, null, 'male', null, '', 'mrmccarthy58@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3314,7 +3316,7 @@
       </c>
       <c r="O41" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addPrimaryMember(@membershipId,'Bryce', 'Hill', 25, null, 'male', null, '', 'bhill@mtech.edu', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addMember(@membershipId,'Bryce', 'Hill', 25, null, 'male', null, '', 'bhill@mtech.edu', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3349,7 +3351,7 @@
       </c>
       <c r="O42" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addPrimaryMember(@membershipId,'Cliff', 'Gade', 25, null, 'male', null, '', 'cliff_gade@hayoo.com', null, null,'Walkerville', '', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addMember(@membershipId,'Cliff', 'Gade', 25, null, 'male', null, '', 'cliff_gade@hayoo.com', null, null,'Walkerville', '', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3387,7 +3389,7 @@
       </c>
       <c r="O43" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addPrimaryMember(@membershipId,'Hansen', 'Velbr', 25, null, 'male', null, '', 'rvehere@mt.gov', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addMember(@membershipId,'Hansen', 'Velbr', 25, null, 'male', null, '', 'rvehere@mt.gov', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3425,7 +3427,7 @@
       </c>
       <c r="O44" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addPrimaryMember(@membershipId,'Pat ', 'Broderick', 25, null, 'male', null, '', 'pwbcanoe99@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-14', '2016-02-14'); call addMember(@membershipId,'Pat ', 'Broderick', 25, null, 'male', null, '', 'pwbcanoe99@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3457,7 +3459,7 @@
       </c>
       <c r="O45" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addPrimaryMember(@membershipId,'Tammy', 'Jonse', 25, null, 'male', null, '', 'sub98@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addMember(@membershipId,'Tammy', 'Jonse', 25, null, 'male', null, '', 'sub98@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3486,7 +3488,7 @@
       </c>
       <c r="O46" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addPrimaryMember(@membershipId,'Ryan', 'Draper', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addMember(@membershipId,'Ryan', 'Draper', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3524,7 +3526,7 @@
       </c>
       <c r="O47" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addPrimaryMember(@membershipId,'Catherine', 'Lace', 25, null, 'male', null, '', 'm53m@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addMember(@membershipId,'Catherine', 'Lace', 25, null, 'male', null, '', 'm53m@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3562,7 +3564,7 @@
       </c>
       <c r="O48" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addPrimaryMember(@membershipId,'Tory', 'Cooper', 25, null, 'male', null, '', 'coopers1305@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addMember(@membershipId,'Tory', 'Cooper', 25, null, 'male', null, '', 'coopers1305@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3600,7 +3602,7 @@
       </c>
       <c r="O49" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addPrimaryMember(@membershipId,'Carly', 'Peach', 25, null, 'male', null, '', 'carlyapeach@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addMember(@membershipId,'Carly', 'Peach', 25, null, 'male', null, '', 'carlyapeach@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3629,7 +3631,7 @@
       </c>
       <c r="O50" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addPrimaryMember(@membershipId,'Bruce/Peggy', 'Graving', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addMember(@membershipId,'Bruce/Peggy', 'Graving', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3667,7 +3669,7 @@
       </c>
       <c r="O51" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addPrimaryMember(@membershipId,'Shilo', 'Van Tatenhove', 25, null, 'male', null, '', 'shilo_v@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addMember(@membershipId,'Shilo', 'Van Tatenhove', 25, null, 'male', null, '', 'shilo_v@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3699,7 +3701,7 @@
       </c>
       <c r="O52" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addPrimaryMember(@membershipId,'Amber', 'Henson', 25, null, 'male', null, '', 'amberjones48@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addMember(@membershipId,'Amber', 'Henson', 25, null, 'male', null, '', 'amberjones48@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3737,7 +3739,7 @@
       </c>
       <c r="O53" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addPrimaryMember(@membershipId,'Denise', 'Hendrix', 25, null, 'male', null, '', 'dhendrix49@outlook.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addMember(@membershipId,'Denise', 'Hendrix', 25, null, 'male', null, '', 'dhendrix49@outlook.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3772,7 +3774,7 @@
       </c>
       <c r="O54" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addPrimaryMember(@membershipId,'Jenny', 'McEwen', 25, null, 'male', null, '', 'jennylmcewen@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addMember(@membershipId,'Jenny', 'McEwen', 25, null, 'male', null, '', 'jennylmcewen@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -3804,7 +3806,7 @@
       </c>
       <c r="O55" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-14', '2016-03-14'); call addPrimaryMember(@membershipId,'Joe', 'Lynch', 25, null, 'male', null, '', 'dtrandal@live.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-14', '2016-03-14'); call addMember(@membershipId,'Joe', 'Lynch', 25, null, 'male', null, '', 'dtrandal@live.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -3842,7 +3844,7 @@
       </c>
       <c r="O56" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-14', '2016-03-14'); call addPrimaryMember(@membershipId,'C', 'Schmalzried', 25, null, 'male', null, '', 'chelseaschmalzried@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-14', '2016-03-14'); call addMember(@membershipId,'C', 'Schmalzried', 25, null, 'male', null, '', 'chelseaschmalzried@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -3871,7 +3873,7 @@
       </c>
       <c r="O57" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addPrimaryMember(@membershipId,'', 'Skinner', 25, null, 'male', null, '', 'jskinner@mtech.edu', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-03-07', '2016-03-07'); call addMember(@membershipId,'', 'Skinner', 25, null, 'male', null, '', 'jskinner@mtech.edu', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -3903,7 +3905,7 @@
       </c>
       <c r="O58" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-06-06', '2016-06-06'); call addPrimaryMember(@membershipId,'Missy', 'Okrusch (Kings Kids)', 25, null, 'male', null, '', 'kingskids0604@hmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-06-06', '2016-06-06'); call addMember(@membershipId,'Missy', 'Okrusch (Kings Kids)', 25, null, 'male', null, '', 'kingskids0604@hmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -3938,7 +3940,7 @@
       </c>
       <c r="O59" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-09-19', '2016-09-19'); call addPrimaryMember(@membershipId,'Judy', 'Evans', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-09-19', '2016-09-19'); call addMember(@membershipId,'Judy', 'Evans', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -3973,7 +3975,7 @@
       </c>
       <c r="O60" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-03', '2016-10-03'); call addPrimaryMember(@membershipId,'Mike', 'Patterson', 25, null, 'male', null, '', 'mhpatterson@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-03', '2016-10-03'); call addMember(@membershipId,'Mike', 'Patterson', 25, null, 'male', null, '', 'mhpatterson@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4005,7 +4007,7 @@
       </c>
       <c r="O61" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-25', '2016-10-25'); call addPrimaryMember(@membershipId,'Dee', 'Wilson', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-25', '2016-10-25'); call addMember(@membershipId,'Dee', 'Wilson', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4042,7 +4044,7 @@
       </c>
       <c r="O62" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-24', '2016-10-24'); call addPrimaryMember(@membershipId,'Judi', 'Schutte', 25, null, 'male', null, '', 'judiliebman', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-24', '2016-10-24'); call addMember(@membershipId,'Judi', 'Schutte', 25, null, 'male', null, '', 'judiliebman', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4080,7 +4082,7 @@
       </c>
       <c r="O63" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-17', '2016-10-17'); call addPrimaryMember(@membershipId,'John', 'Babcock', 25, null, 'male', null, '', 'jbabcock@wet-llc.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-17', '2016-10-17'); call addMember(@membershipId,'John', 'Babcock', 25, null, 'male', null, '', 'jbabcock@wet-llc.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4118,7 +4120,7 @@
       </c>
       <c r="O64" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-03', '2016-10-03'); call addPrimaryMember(@membershipId,'Lee', 'Good', 25, null, 'male', null, '', 'tssmail@tssmt.net', null, null,'Whitehall', '', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-03', '2016-10-03'); call addMember(@membershipId,'Lee', 'Good', 25, null, 'male', null, '', 'tssmail@tssmt.net', null, null,'Whitehall', '', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4156,7 +4158,7 @@
       </c>
       <c r="O65" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-03', '2016-10-03'); call addPrimaryMember(@membershipId,'Patrick', 'Broderick', 25, null, 'male', null, '', 'pwbcanoe99@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-03', '2016-10-03'); call addMember(@membershipId,'Patrick', 'Broderick', 25, null, 'male', null, '', 'pwbcanoe99@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4194,7 +4196,7 @@
       </c>
       <c r="O66" t="str">
         <f t="shared" si="2"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-09-30', '2016-09-30'); call addPrimaryMember(@membershipId,'Mary Kay', 'Craig', 25, null, 'male', null, '', 'marykathleencraig@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-09-30', '2016-09-30'); call addMember(@membershipId,'Mary Kay', 'Craig', 25, null, 'male', null, '', 'marykathleencraig@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4228,8 +4230,8 @@
         <v>2016-12-05</v>
       </c>
       <c r="O67" t="str">
-        <f t="shared" ref="O67:O130" si="5">_xlfn.CONCAT("call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '", L67, "', '", M67, "'); call addPrimaryMember(@membershipId,'", B67, "', '", A67, "', 25, null, 'male', null, '", J67, "', '", H67, "', null, null,'", D67, "', '", C67, "', 'MT');")</f>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-12-05', '2016-12-05'); call addPrimaryMember(@membershipId,'Titus', 'Bergren', 25, null, 'male', null, '', 'titusbergren@gmail.com', null, null,'', '59701', 'MT');</v>
+        <f t="shared" ref="O67:O130" si="5">_xlfn.CONCAT("call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '", L67, "', '", M67, "'); call addMember(@membershipId,'", B67, "', '", A67, "', 25, null, 'male', null, '", J67, "', '", H67, "', null, null,'", D67, "', '", C67, "', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);")</f>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-12-05', '2016-12-05'); call addMember(@membershipId,'Titus', 'Bergren', 25, null, 'male', null, '', 'titusbergren@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4264,7 +4266,7 @@
       </c>
       <c r="O68" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-01-21', '2016-01-21'); call addPrimaryMember(@membershipId,'Alicia', 'Kachmavik', 25, null, 'male', null, '', 'aliciawheeler@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-01-21', '2016-01-21'); call addMember(@membershipId,'Alicia', 'Kachmavik', 25, null, 'male', null, '', 'aliciawheeler@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4299,7 +4301,7 @@
       </c>
       <c r="O69" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-11-21', '2016-11-21'); call addPrimaryMember(@membershipId,'Elizabeth', 'Drew', 25, null, 'male', null, '', 'birddrew222@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-11-21', '2016-11-21'); call addMember(@membershipId,'Elizabeth', 'Drew', 25, null, 'male', null, '', 'birddrew222@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4331,7 +4333,7 @@
       </c>
       <c r="O70" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-12-19', '2016-12-19'); call addPrimaryMember(@membershipId,'Pate', 'Briggs', 25, null, 'male', null, '', '', null, null,'Anaconda', '59711', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-12-19', '2016-12-19'); call addMember(@membershipId,'Pate', 'Briggs', 25, null, 'male', null, '', '', null, null,'Anaconda', '59711', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4366,7 +4368,7 @@
       </c>
       <c r="O71" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-12-12', '2016-12-12'); call addPrimaryMember(@membershipId,'Ben/Jess', 'Carr', 25, null, 'male', null, '', 'jdrewnumerouno@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-12-12', '2016-12-12'); call addMember(@membershipId,'Ben/Jess', 'Carr', 25, null, 'male', null, '', 'jdrewnumerouno@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="72" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4401,7 +4403,7 @@
       </c>
       <c r="O72" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-12-12', '2016-12-12'); call addPrimaryMember(@membershipId,'Sabina', 'Pate-Terry', 25, null, 'male', null, '', 'anatoart@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-12-12', '2016-12-12'); call addMember(@membershipId,'Sabina', 'Pate-Terry', 25, null, 'male', null, '', 'anatoart@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4436,7 +4438,7 @@
       </c>
       <c r="O73" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-01-23', '2016-01-23'); call addPrimaryMember(@membershipId,'Ashley', 'Neighbor', 25, null, 'male', null, '', 'ashleyannneighbor@outlook.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-01-23', '2016-01-23'); call addMember(@membershipId,'Ashley', 'Neighbor', 25, null, 'male', null, '', 'ashleyannneighbor@outlook.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="74" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4468,7 +4470,7 @@
       </c>
       <c r="O74" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addPrimaryMember(@membershipId,'Mike', 'Bordwin', 25, null, 'male', null, '', 'mbordwin@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-11', '2016-04-11'); call addMember(@membershipId,'Mike', 'Bordwin', 25, null, 'male', null, '', 'mbordwin@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="75" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4500,7 +4502,7 @@
       </c>
       <c r="O75" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-02-13', '2017-02-13'); call addPrimaryMember(@membershipId,'Allison', 'Andersen', 25, null, 'male', null, '', 'phippsqllijo@juno.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-02-13', '2017-02-13'); call addMember(@membershipId,'Allison', 'Andersen', 25, null, 'male', null, '', 'phippsqllijo@juno.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="76" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4532,7 +4534,7 @@
       </c>
       <c r="O76" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-30', '2017-04-30'); call addPrimaryMember(@membershipId,'Darla', 'Moran', 25, null, 'male', null, '', 'dmorqn51@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-30', '2017-04-30'); call addMember(@membershipId,'Darla', 'Moran', 25, null, 'male', null, '', 'dmorqn51@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4564,7 +4566,7 @@
       </c>
       <c r="O77" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-20', '2017-04-20'); call addPrimaryMember(@membershipId,'Theron', 'Wilson', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-20', '2017-04-20'); call addMember(@membershipId,'Theron', 'Wilson', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4596,7 +4598,7 @@
       </c>
       <c r="O78" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-17', '2017-04-17'); call addPrimaryMember(@membershipId,'Mike', 'Bordwin', 25, null, 'male', null, '', 'mbordwin@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-17', '2017-04-17'); call addMember(@membershipId,'Mike', 'Bordwin', 25, null, 'male', null, '', 'mbordwin@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4628,7 +4630,7 @@
       </c>
       <c r="O79" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-16', '2017-04-16'); call addPrimaryMember(@membershipId,'Becky', 'Fisk', 25, null, 'male', null, '', 'fiskfam4@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-16', '2017-04-16'); call addMember(@membershipId,'Becky', 'Fisk', 25, null, 'male', null, '', 'fiskfam4@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4663,7 +4665,7 @@
       </c>
       <c r="O80" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-09', '2017-04-09'); call addPrimaryMember(@membershipId,'Gary', 'Wyss', 25, null, 'male', null, '', 'wyssl@aol.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-09', '2017-04-09'); call addMember(@membershipId,'Gary', 'Wyss', 25, null, 'male', null, '', 'wyssl@aol.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4698,7 +4700,7 @@
       </c>
       <c r="O81" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-09', '2017-04-09'); call addPrimaryMember(@membershipId,'C', 'Schmalzried', 25, null, 'male', null, '', 'chelseaschmalzried@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-04-09', '2017-04-09'); call addMember(@membershipId,'C', 'Schmalzried', 25, null, 'male', null, '', 'chelseaschmalzried@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4736,7 +4738,7 @@
       </c>
       <c r="O82" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-05-21', '2017-05-21'); call addPrimaryMember(@membershipId,'Dave', 'McCarthy', 25, null, 'male', null, '', 'smelter01@gmail.com', null, null,'Anaconda', '59711', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-05-21', '2017-05-21'); call addMember(@membershipId,'Dave', 'McCarthy', 25, null, 'male', null, '', 'smelter01@gmail.com', null, null,'Anaconda', '59711', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4771,7 +4773,7 @@
       </c>
       <c r="O83" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-05-21', '2017-05-21'); call addPrimaryMember(@membershipId,'Lucy', 'Ednie', 25, null, 'male', null, '', 'lucysupernurse@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-05-21', '2017-05-21'); call addMember(@membershipId,'Lucy', 'Ednie', 25, null, 'male', null, '', 'lucysupernurse@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4806,7 +4808,7 @@
       </c>
       <c r="O84" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-05-21', '2017-05-21'); call addPrimaryMember(@membershipId,'Jason', 'Korst', 25, null, 'male', null, '', 'korsty@hotmail.com', null, null,'Whitehall', '59759', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-05-21', '2017-05-21'); call addMember(@membershipId,'Jason', 'Korst', 25, null, 'male', null, '', 'korsty@hotmail.com', null, null,'Whitehall', '59759', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4841,7 +4843,7 @@
       </c>
       <c r="O85" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-05-21', '2017-05-21'); call addPrimaryMember(@membershipId,'Rozanne', 'Conley', 25, null, 'male', null, '', 'roxannec1969@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-05-21', '2017-05-21'); call addMember(@membershipId,'Rozanne', 'Conley', 25, null, 'male', null, '', 'roxannec1969@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="86" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4870,7 +4872,7 @@
       </c>
       <c r="O86" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-05-07', '2017-05-07'); call addPrimaryMember(@membershipId,'JJ', 'Bestgen', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-05-07', '2017-05-07'); call addMember(@membershipId,'JJ', 'Bestgen', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="87" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4905,7 +4907,7 @@
       </c>
       <c r="O87" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-03-12', '2017-03-12'); call addPrimaryMember(@membershipId,'Rick', 'Jordan', 25, null, 'male', null, '', 'rjordan@barrick.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-03-12', '2017-03-12'); call addMember(@membershipId,'Rick', 'Jordan', 25, null, 'male', null, '', 'rjordan@barrick.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4939,7 +4941,7 @@
       </c>
       <c r="O88" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-03-12', '2017-03-12'); call addPrimaryMember(@membershipId,'Mike', 'Nasheim', 25, null, 'male', null, '', 'san21456@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-03-12', '2017-03-12'); call addMember(@membershipId,'Mike', 'Nasheim', 25, null, 'male', null, '', 'san21456@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -4968,7 +4970,7 @@
       </c>
       <c r="O89" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Alyssa', 'Creighton', 25, null, 'male', null, '', '', null, null,'Dillon', '59725', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Alyssa', 'Creighton', 25, null, 'male', null, '', '', null, null,'Dillon', '59725', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="90" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5006,7 +5008,7 @@
       </c>
       <c r="O90" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-02-13', '2017-02-13'); call addPrimaryMember(@membershipId,'Lesley', 'Holman', 25, null, 'male', null, '', 'holmanla@butte.k12.mt.us ', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-02-13', '2017-02-13'); call addMember(@membershipId,'Lesley', 'Holman', 25, null, 'male', null, '', 'holmanla@butte.k12.mt.us ', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="91" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5041,7 +5043,7 @@
       </c>
       <c r="O91" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-19', '2017-01-19'); call addPrimaryMember(@membershipId,'Gene/Tammy', 'Jense', 25, null, 'male', null, '', 'sub90@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-19', '2017-01-19'); call addMember(@membershipId,'Gene/Tammy', 'Jense', 25, null, 'male', null, '', 'sub90@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="92" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5073,7 +5075,7 @@
       </c>
       <c r="O92" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-19', '2017-01-19'); call addPrimaryMember(@membershipId,'', 'Skinner', 25, null, 'male', null, '', 'wgskinn@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-19', '2017-01-19'); call addMember(@membershipId,'', 'Skinner', 25, null, 'male', null, '', 'wgskinn@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5105,7 +5107,7 @@
       </c>
       <c r="O93" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addPrimaryMember(@membershipId,'', 'Callaghan', 25, null, 'male', null, '', 'callaghanwe@butte.k12.mt.us', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addMember(@membershipId,'', 'Callaghan', 25, null, 'male', null, '', 'callaghanwe@butte.k12.mt.us', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5140,7 +5142,7 @@
       </c>
       <c r="O94" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addPrimaryMember(@membershipId,'Chandra', 'Duran', 25, null, 'male', null, '', 'chandraduran@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addMember(@membershipId,'Chandra', 'Duran', 25, null, 'male', null, '', 'chandraduran@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="95" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5175,7 +5177,7 @@
       </c>
       <c r="O95" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addPrimaryMember(@membershipId,'Shella', 'Capaccia', 25, null, 'male', null, '', 'scapoccia@mttech.edu', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addMember(@membershipId,'Shella', 'Capaccia', 25, null, 'male', null, '', 'scapoccia@mttech.edu', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="96" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5210,7 +5212,7 @@
       </c>
       <c r="O96" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-23', '2017-11-23'); call addPrimaryMember(@membershipId,'Tim', 'Lynch', 25, null, 'male', null, '', 'tlynch@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-23', '2017-11-23'); call addMember(@membershipId,'Tim', 'Lynch', 25, null, 'male', null, '', 'tlynch@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="97" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5245,7 +5247,7 @@
       </c>
       <c r="O97" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addPrimaryMember(@membershipId,'Tracy', 'Cannon', 25, null, 'male', null, '', 'tracyc-tech@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addMember(@membershipId,'Tracy', 'Cannon', 25, null, 'male', null, '', 'tracyc-tech@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="98" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5280,7 +5282,7 @@
       </c>
       <c r="O98" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addPrimaryMember(@membershipId,'Tina', 'Pantano', 25, null, 'male', null, '', 'tmpantano@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addMember(@membershipId,'Tina', 'Pantano', 25, null, 'male', null, '', 'tmpantano@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="99" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5315,7 +5317,7 @@
       </c>
       <c r="O99" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addPrimaryMember(@membershipId,'Sheilah', 'VIncent', 25, null, 'male', null, '', 'elvisbutte@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addMember(@membershipId,'Sheilah', 'VIncent', 25, null, 'male', null, '', 'elvisbutte@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="100" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5341,7 +5343,7 @@
       </c>
       <c r="O100" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addPrimaryMember(@membershipId,'', 'Brady', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-23', '2017-01-23'); call addMember(@membershipId,'', 'Brady', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="101" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5376,7 +5378,7 @@
       </c>
       <c r="O101" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-30', '2017-01-30'); call addPrimaryMember(@membershipId,'Evan', 'Barrett', 25, null, 'male', null, '', 'evanbutte@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-30', '2017-01-30'); call addMember(@membershipId,'Evan', 'Barrett', 25, null, 'male', null, '', 'evanbutte@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="102" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5414,7 +5416,7 @@
       </c>
       <c r="O102" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-09-23', '2017-09-23'); call addPrimaryMember(@membershipId,'Larry', 'Hoffman', 25, null, 'male', null, '', 'hardrock4800@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-09-23', '2017-09-23'); call addMember(@membershipId,'Larry', 'Hoffman', 25, null, 'male', null, '', 'hardrock4800@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="103" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5452,7 +5454,7 @@
       </c>
       <c r="O103" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-09-24', '2017-09-24'); call addPrimaryMember(@membershipId,'Cormic', 'Sletten', 25, null, 'male', null, '', 'acombo@bldc.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-09-24', '2017-09-24'); call addMember(@membershipId,'Cormic', 'Sletten', 25, null, 'male', null, '', 'acombo@bldc.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="104" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5487,7 +5489,7 @@
       </c>
       <c r="O104" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-09-25', '2017-09-25'); call addPrimaryMember(@membershipId,'', 'Ball', 25, null, 'male', null, '', 'ball7134@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-09-25', '2017-09-25'); call addMember(@membershipId,'', 'Ball', 25, null, 'male', null, '', 'ball7134@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="105" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5522,7 +5524,7 @@
       </c>
       <c r="O105" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-01', '2017-10-01'); call addPrimaryMember(@membershipId,'Dolores', 'Cooney', 25, null, 'male', null, '', 'dcooney@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-01', '2017-10-01'); call addMember(@membershipId,'Dolores', 'Cooney', 25, null, 'male', null, '', 'dcooney@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="106" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5560,7 +5562,7 @@
       </c>
       <c r="O106" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addPrimaryMember(@membershipId,'Rounds', 'Shuttlesworth', 25, null, 'male', null, '', 'h/rounds@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addMember(@membershipId,'Rounds', 'Shuttlesworth', 25, null, 'male', null, '', 'h/rounds@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="107" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5598,7 +5600,7 @@
       </c>
       <c r="O107" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addPrimaryMember(@membershipId,'Avi', 'Masters', 25, null, 'male', null, '', 'mmasters@mtech.edu', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addMember(@membershipId,'Avi', 'Masters', 25, null, 'male', null, '', 'mmasters@mtech.edu', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="108" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5636,7 +5638,7 @@
       </c>
       <c r="O108" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addPrimaryMember(@membershipId,'Tera', 'Ryan', 25, null, 'male', null, '', 'bryan@mtech.edu', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addMember(@membershipId,'Tera', 'Ryan', 25, null, 'male', null, '', 'bryan@mtech.edu', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="109" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5674,7 +5676,7 @@
       </c>
       <c r="O109" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addPrimaryMember(@membershipId,'Asna', 'Henne/capocca', 25, null, 'male', null, '', 'scapoccia@mtech.edu', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addMember(@membershipId,'Asna', 'Henne/capocca', 25, null, 'male', null, '', 'scapoccia@mtech.edu', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="110" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5709,7 +5711,7 @@
       </c>
       <c r="O110" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addPrimaryMember(@membershipId,'Terry', 'Pate', 25, null, 'male', null, '', 'anatoart@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addMember(@membershipId,'Terry', 'Pate', 25, null, 'male', null, '', 'anatoart@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="111" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5744,7 +5746,7 @@
       </c>
       <c r="O111" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addPrimaryMember(@membershipId,'Barbie', 'Huber', 25, null, 'male', null, '', 'barbiehuber@hotmail.com', null, null,'Bozeman', '', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-08', '2017-10-08'); call addMember(@membershipId,'Barbie', 'Huber', 25, null, 'male', null, '', 'barbiehuber@hotmail.com', null, null,'Bozeman', '', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="112" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5782,7 +5784,7 @@
       </c>
       <c r="O112" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-14', '2017-10-14'); call addPrimaryMember(@membershipId,'Kelly', 'Thatcher', 25, null, 'male', null, '', 'jayhubber24@aol.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-14', '2017-10-14'); call addMember(@membershipId,'Kelly', 'Thatcher', 25, null, 'male', null, '', 'jayhubber24@aol.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="113" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5820,7 +5822,7 @@
       </c>
       <c r="O113" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-15', '2017-10-15'); call addPrimaryMember(@membershipId,'Amber/Dennis', 'Osterman', 25, null, 'male', null, '', 'osterwoman@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-15', '2017-10-15'); call addMember(@membershipId,'Amber/Dennis', 'Osterman', 25, null, 'male', null, '', 'osterwoman@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="114" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5858,7 +5860,7 @@
       </c>
       <c r="O114" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-15', '2017-10-15'); call addPrimaryMember(@membershipId,'Jeannine', 'Boyle', 25, null, 'male', null, '', 'jeboylesr@sbcglobal.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-15', '2017-10-15'); call addMember(@membershipId,'Jeannine', 'Boyle', 25, null, 'male', null, '', 'jeboylesr@sbcglobal.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="115" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5896,7 +5898,7 @@
       </c>
       <c r="O115" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-15', '2017-10-15'); call addPrimaryMember(@membershipId,'Ottolini', 'Messukri', 25, null, 'male', null, '', 'aottolinimessuri@mtech.edu', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-15', '2017-10-15'); call addMember(@membershipId,'Ottolini', 'Messukri', 25, null, 'male', null, '', 'aottolinimessuri@mtech.edu', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="116" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5931,7 +5933,7 @@
       </c>
       <c r="O116" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-22', '2017-10-22'); call addPrimaryMember(@membershipId,'', 'Vavruska', 25, null, 'male', null, '', 'invavruska@bresnan.net', null, null,'Helena', '59635', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-22', '2017-10-22'); call addMember(@membershipId,'', 'Vavruska', 25, null, 'male', null, '', 'invavruska@bresnan.net', null, null,'Helena', '59635', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="117" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5960,7 +5962,7 @@
       </c>
       <c r="O117" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-29', '2017-10-29'); call addPrimaryMember(@membershipId,'Robin', 'Johnson', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-29', '2017-10-29'); call addMember(@membershipId,'Robin', 'Johnson', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="118" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -5998,7 +6000,7 @@
       </c>
       <c r="O118" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-29', '2017-10-29'); call addPrimaryMember(@membershipId,'Melissa', 'Kump', 25, null, 'male', null, '', 'melissaann49@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-29', '2017-10-29'); call addMember(@membershipId,'Melissa', 'Kump', 25, null, 'male', null, '', 'melissaann49@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="119" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6036,7 +6038,7 @@
       </c>
       <c r="O119" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-29', '2017-10-29'); call addPrimaryMember(@membershipId,'Patrick', 'Broderick', 25, null, 'male', null, '', 'pwbcanoe99@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-10-29', '2017-10-29'); call addMember(@membershipId,'Patrick', 'Broderick', 25, null, 'male', null, '', 'pwbcanoe99@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="120" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6074,7 +6076,7 @@
       </c>
       <c r="O120" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-05', '2017-11-05'); call addPrimaryMember(@membershipId,'Shane/Heather', 'Davis', 25, null, 'male', null, '', 'hmdavisdum@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-05', '2017-11-05'); call addMember(@membershipId,'Shane/Heather', 'Davis', 25, null, 'male', null, '', 'hmdavisdum@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="121" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6112,7 +6114,7 @@
       </c>
       <c r="O121" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-05', '2017-11-05'); call addPrimaryMember(@membershipId,'JoAnna', 'Buchholz', 25, null, 'male', null, '', 'joanna_buchholz@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-05', '2017-11-05'); call addMember(@membershipId,'JoAnna', 'Buchholz', 25, null, 'male', null, '', 'joanna_buchholz@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="122" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6153,7 +6155,7 @@
       </c>
       <c r="O122" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-05', '2017-11-05'); call addPrimaryMember(@membershipId,'Robert', 'Moler', 25, null, 'male', null, '', 'robertmoler@gmail.com', null, null,'Helena', '59601', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-05', '2017-11-05'); call addMember(@membershipId,'Robert', 'Moler', 25, null, 'male', null, '', 'robertmoler@gmail.com', null, null,'Helena', '59601', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="123" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6182,7 +6184,7 @@
       </c>
       <c r="O123" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-12', '2017-11-12'); call addPrimaryMember(@membershipId,'Oly', 'Petersen', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-12', '2017-11-12'); call addMember(@membershipId,'Oly', 'Petersen', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="124" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6217,7 +6219,7 @@
       </c>
       <c r="O124" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-26', '2017-11-26'); call addPrimaryMember(@membershipId,'Marlene', 'Worthon', 25, null, 'male', null, '', 'marlenegreen3@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-26', '2017-11-26'); call addMember(@membershipId,'Marlene', 'Worthon', 25, null, 'male', null, '', 'marlenegreen3@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="125" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6249,7 +6251,7 @@
       </c>
       <c r="O125" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-26', '2017-11-26'); call addPrimaryMember(@membershipId,'Bryan/Mandy', 'Armstrong', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-11-26', '2017-11-26'); call addMember(@membershipId,'Bryan/Mandy', 'Armstrong', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="126" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6284,7 +6286,7 @@
       </c>
       <c r="O126" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-22', '2018-04-22'); call addPrimaryMember(@membershipId,'', 'Walsh', 25, null, 'male', null, '', 'mlwalsh@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-22', '2018-04-22'); call addMember(@membershipId,'', 'Walsh', 25, null, 'male', null, '', 'mlwalsh@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="127" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6319,7 +6321,7 @@
       </c>
       <c r="O127" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-03', '2018-06-03'); call addPrimaryMember(@membershipId,'Glenn', 'Brackett', 25, null, 'male', null, '', 'glencris@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-03', '2018-06-03'); call addMember(@membershipId,'Glenn', 'Brackett', 25, null, 'male', null, '', 'glencris@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="128" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6351,7 +6353,7 @@
       </c>
       <c r="O128" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-03', '2018-06-03'); call addPrimaryMember(@membershipId,'', 'Schulte', 25, null, 'male', null, '', 'gregoryjamesschulte@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-03', '2018-06-03'); call addMember(@membershipId,'', 'Schulte', 25, null, 'male', null, '', 'gregoryjamesschulte@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="129" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6383,7 +6385,7 @@
       </c>
       <c r="O129" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-10', '2018-06-10'); call addPrimaryMember(@membershipId,'Carol', 'Smith', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-10', '2018-06-10'); call addMember(@membershipId,'Carol', 'Smith', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="130" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6421,7 +6423,7 @@
       </c>
       <c r="O130" t="str">
         <f t="shared" si="5"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-10', '2018-06-10'); call addPrimaryMember(@membershipId,'Gayle', 'Nicholls', 25, null, 'male', null, '', 'gnicholls@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-10', '2018-06-10'); call addMember(@membershipId,'Gayle', 'Nicholls', 25, null, 'male', null, '', 'gnicholls@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="131" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6458,8 +6460,8 @@
         <v>2018-06-17</v>
       </c>
       <c r="O131" t="str">
-        <f t="shared" ref="O131:O189" si="8">_xlfn.CONCAT("call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '", L131, "', '", M131, "'); call addPrimaryMember(@membershipId,'", B131, "', '", A131, "', 25, null, 'male', null, '", J131, "', '", H131, "', null, null,'", D131, "', '", C131, "', 'MT');")</f>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-17', '2018-06-17'); call addPrimaryMember(@membershipId,'Dolores', 'Cooney', 25, null, 'male', null, '', 'dcooney@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <f t="shared" ref="O131:O189" si="8">_xlfn.CONCAT("call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '", L131, "', '", M131, "'); call addMember(@membershipId,'", B131, "', '", A131, "', 25, null, 'male', null, '", J131, "', '", H131, "', null, null,'", D131, "', '", C131, "', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);")</f>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-17', '2018-06-17'); call addMember(@membershipId,'Dolores', 'Cooney', 25, null, 'male', null, '', 'dcooney@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="132" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6494,7 +6496,7 @@
       </c>
       <c r="O132" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-17', '2018-06-17'); call addPrimaryMember(@membershipId,'Fred/Bev', 'Hartline', 25, null, 'male', null, '', 'fbhartl@earthlink.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-17', '2018-06-17'); call addMember(@membershipId,'Fred/Bev', 'Hartline', 25, null, 'male', null, '', 'fbhartl@earthlink.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="133" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6532,7 +6534,7 @@
       </c>
       <c r="O133" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-24', '2018-06-24'); call addPrimaryMember(@membershipId,'Missy', 'Okrusch', 25, null, 'male', null, '', 'kingskids0604@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-24', '2018-06-24'); call addMember(@membershipId,'Missy', 'Okrusch', 25, null, 'male', null, '', 'kingskids0604@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="134" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6567,7 +6569,7 @@
       </c>
       <c r="O134" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-24', '2018-06-24'); call addPrimaryMember(@membershipId,'Decia', 'Newby', 25, null, 'male', null, '', 'jaconandecia@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-24', '2018-06-24'); call addMember(@membershipId,'Decia', 'Newby', 25, null, 'male', null, '', 'jaconandecia@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="135" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6599,7 +6601,7 @@
       </c>
       <c r="O135" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-24', '2018-06-24'); call addPrimaryMember(@membershipId,'', 'Naglsetty', 25, null, 'male', null, '', 'jyoti.nagisetty@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-06-24', '2018-06-24'); call addMember(@membershipId,'', 'Naglsetty', 25, null, 'male', null, '', 'jyoti.nagisetty@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="136" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6631,7 +6633,7 @@
       </c>
       <c r="O136" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2027-06-24', '2028-06-24'); call addPrimaryMember(@membershipId,'', 'Jamison', 25, null, 'male', null, '', 'shawnajamison@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2027-06-24', '2028-06-24'); call addMember(@membershipId,'', 'Jamison', 25, null, 'male', null, '', 'shawnajamison@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="137" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6669,7 +6671,7 @@
       </c>
       <c r="O137" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-28', '2018-01-28'); call addPrimaryMember(@membershipId,'Allison', 'Andersen', 25, null, 'male', null, '', 'phippsallijoa@juno.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-28', '2018-01-28'); call addMember(@membershipId,'Allison', 'Andersen', 25, null, 'male', null, '', 'phippsallijoa@juno.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="138" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6707,7 +6709,7 @@
       </c>
       <c r="O138" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-02-04', '2018-02-04'); call addPrimaryMember(@membershipId,'Ben', 'Clark', 25, null, 'male', null, '', 'lineman669@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-02-04', '2018-02-04'); call addMember(@membershipId,'Ben', 'Clark', 25, null, 'male', null, '', 'lineman669@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="139" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6742,7 +6744,7 @@
       </c>
       <c r="O139" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-02-04', '2018-02-04'); call addPrimaryMember(@membershipId,'', 'Hasslers', 25, null, 'male', null, '', 'kpowley@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-02-04', '2018-02-04'); call addMember(@membershipId,'', 'Hasslers', 25, null, 'male', null, '', 'kpowley@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="140" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6777,7 +6779,7 @@
       </c>
       <c r="O140" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-14', '2018-01-14'); call addPrimaryMember(@membershipId,'Gayle', 'Nicholls', 25, null, 'male', null, '', 'gnicholls@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-14', '2018-01-14'); call addMember(@membershipId,'Gayle', 'Nicholls', 25, null, 'male', null, '', 'gnicholls@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="141" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6815,7 +6817,7 @@
       </c>
       <c r="O141" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-14', '2018-01-14'); call addPrimaryMember(@membershipId,'Catherine', 'Lace', 25, null, 'male', null, '', 'm53m@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-14', '2018-01-14'); call addMember(@membershipId,'Catherine', 'Lace', 25, null, 'male', null, '', 'm53m@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="142" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6853,7 +6855,7 @@
       </c>
       <c r="O142" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-14', '2018-01-14'); call addPrimaryMember(@membershipId,'Havilah', 'Hill', 25, null, 'male', null, '', 'havilahhill@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-14', '2018-01-14'); call addMember(@membershipId,'Havilah', 'Hill', 25, null, 'male', null, '', 'havilahhill@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="143" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6885,7 +6887,7 @@
       </c>
       <c r="O143" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Cormic', 'Sletten', 25, null, 'male', null, '', 'acombo@bldc.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Cormic', 'Sletten', 25, null, 'male', null, '', 'acombo@bldc.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="144" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6923,7 +6925,7 @@
       </c>
       <c r="O144" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-17', '2018-01-17'); call addPrimaryMember(@membershipId,'Paige', 'Thompson', 25, null, 'male', null, '', 'mthompson1828@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-17', '2018-01-17'); call addMember(@membershipId,'Paige', 'Thompson', 25, null, 'male', null, '', 'mthompson1828@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="145" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6961,7 +6963,7 @@
       </c>
       <c r="O145" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-02-04', '2018-02-04'); call addPrimaryMember(@membershipId,'Tyler', 'Storey', 25, null, 'male', null, '', 'xtyler.storeyx@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-02-04', '2018-02-04'); call addMember(@membershipId,'Tyler', 'Storey', 25, null, 'male', null, '', 'xtyler.storeyx@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="146" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -6999,7 +7001,7 @@
       </c>
       <c r="O146" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-08', '2018-04-08'); call addPrimaryMember(@membershipId,'Kim', 'Ward', 25, null, 'male', null, '', 'wardlk4@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-08', '2018-04-08'); call addMember(@membershipId,'Kim', 'Ward', 25, null, 'male', null, '', 'wardlk4@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="147" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7034,7 +7036,7 @@
       </c>
       <c r="O147" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-08', '2018-04-08'); call addPrimaryMember(@membershipId,'J', 'Ball', 25, null, 'male', null, '', 'ball7134@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-08', '2018-04-08'); call addMember(@membershipId,'J', 'Ball', 25, null, 'male', null, '', 'ball7134@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="148" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7066,7 +7068,7 @@
       </c>
       <c r="O148" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-08', '2018-04-08'); call addPrimaryMember(@membershipId,'', 'Welker', 25, null, 'male', null, '', 'nicwelker@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-08', '2018-04-08'); call addMember(@membershipId,'', 'Welker', 25, null, 'male', null, '', 'nicwelker@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="149" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7101,7 +7103,7 @@
       </c>
       <c r="O149" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-05-17', '2018-05-17'); call addPrimaryMember(@membershipId,'', 'Cyr', 25, null, 'male', null, '', 'cyr61us@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-05-17', '2018-05-17'); call addMember(@membershipId,'', 'Cyr', 25, null, 'male', null, '', 'cyr61us@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="150" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7136,7 +7138,7 @@
       </c>
       <c r="O150" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-05-20', '2018-05-20'); call addPrimaryMember(@membershipId,'John', 'Babcock', 25, null, 'male', null, '', 'johnbabcock@hotmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-05-20', '2018-05-20'); call addMember(@membershipId,'John', 'Babcock', 25, null, 'male', null, '', 'johnbabcock@hotmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="151" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7174,7 +7176,7 @@
       </c>
       <c r="O151" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-05-27', '2018-05-27'); call addPrimaryMember(@membershipId,'Fallen', 'Bennett', 25, null, 'male', null, '', 'maggie.pierce@youthdynamics.org', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-05-27', '2018-05-27'); call addMember(@membershipId,'Fallen', 'Bennett', 25, null, 'male', null, '', 'maggie.pierce@youthdynamics.org', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="152" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7206,7 +7208,7 @@
       </c>
       <c r="O152" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Dave', 'Holman', 25, null, 'male', null, '', 'jetdog23@aol.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Dave', 'Holman', 25, null, 'male', null, '', 'jetdog23@aol.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="153" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7232,7 +7234,7 @@
       </c>
       <c r="O153" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Megan', 'O'keefe', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Megan', 'O'keefe', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="154" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7255,7 +7257,7 @@
       </c>
       <c r="O154" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Ryan', 'Mullcahy', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Ryan', 'Mullcahy', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="155" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7284,7 +7286,7 @@
       </c>
       <c r="O155" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-18', '2016-04-18'); call addPrimaryMember(@membershipId,'Todd/Mitzi', 'Leibrand', 25, null, 'male', null, '', '', null, null,'', '59421', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-04-18', '2016-04-18'); call addMember(@membershipId,'Todd/Mitzi', 'Leibrand', 25, null, 'male', null, '', '', null, null,'', '59421', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="156" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7317,7 +7319,7 @@
       </c>
       <c r="O156" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Lee', 'Tierney', 25, null, 'male', null, '', 'ltiern8@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Lee', 'Tierney', 25, null, 'male', null, '', 'ltiern8@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="157" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7349,7 +7351,7 @@
       </c>
       <c r="O157" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Nate', 'Watson', 25, null, 'male', null, '', 'nate.watson82@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Nate', 'Watson', 25, null, 'male', null, '', 'nate.watson82@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="158" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7378,7 +7380,7 @@
       </c>
       <c r="O158" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Maggie', 'Ferko', 25, null, 'male', null, '', 'margaretferko@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Maggie', 'Ferko', 25, null, 'male', null, '', 'margaretferko@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="159" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7407,7 +7409,7 @@
       </c>
       <c r="O159" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Larry/Nancy', 'Hoffman', 25, null, 'male', null, '', 'hardrock4800@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Larry/Nancy', 'Hoffman', 25, null, 'male', null, '', 'hardrock4800@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="160" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7436,7 +7438,7 @@
       </c>
       <c r="O160" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Laura', 'Moore', 25, null, 'male', null, '', 'laurazorn3@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Laura', 'Moore', 25, null, 'male', null, '', 'laurazorn3@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="161" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7465,7 +7467,7 @@
       </c>
       <c r="O161" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Hilary', 'Risser', 25, null, 'male', null, '', 'hsrisser@mac.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Hilary', 'Risser', 25, null, 'male', null, '', 'hsrisser@mac.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="162" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7497,7 +7499,7 @@
       </c>
       <c r="O162" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'John', 'Tomich', 25, null, 'male', null, '', 'jtomich@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'John', 'Tomich', 25, null, 'male', null, '', 'jtomich@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="163" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7529,7 +7531,7 @@
       </c>
       <c r="O163" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Pam', 'Dazby-Cote', 25, null, 'male', null, '', 'pamcote114@msn.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Pam', 'Dazby-Cote', 25, null, 'male', null, '', 'pamcote114@msn.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="164" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7564,7 +7566,7 @@
       </c>
       <c r="O164" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'J.', 'Boyer', 25, null, 'male', null, '', 'jamieboyer1130@hotmail.com', null, null,'Anaconda', '59711', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'J.', 'Boyer', 25, null, 'male', null, '', 'jamieboyer1130@hotmail.com', null, null,'Anaconda', '59711', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="165" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7599,7 +7601,7 @@
       </c>
       <c r="O165" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addPrimaryMember(@membershipId,'Ben', 'Rapkod', 25, null, 'male', null, '', 'claudiarap59701@msn.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addMember(@membershipId,'Ben', 'Rapkod', 25, null, 'male', null, '', 'claudiarap59701@msn.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="166" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7628,7 +7630,7 @@
       </c>
       <c r="O166" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Susan', 'Callaghan', 25, null, 'male', null, '', 'sjcmt2003@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Susan', 'Callaghan', 25, null, 'male', null, '', 'sjcmt2003@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="167" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7663,7 +7665,7 @@
       </c>
       <c r="O167" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addPrimaryMember(@membershipId,'Taryn', 'Calderon', 25, null, 'male', null, '', 'tarynj21691@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-02-28', '2016-02-28'); call addMember(@membershipId,'Taryn', 'Calderon', 25, null, 'male', null, '', 'tarynj21691@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="168" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7695,7 +7697,7 @@
       </c>
       <c r="O168" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Allison', 'Andersen', 25, null, 'male', null, '', 'phippsallijo@juno.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Allison', 'Andersen', 25, null, 'male', null, '', 'phippsallijo@juno.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="169" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7730,7 +7732,7 @@
       </c>
       <c r="O169" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-24', '2016-10-24'); call addPrimaryMember(@membershipId,'Chrissy', 'Hadley', 25, null, 'male', null, '', 'clhadley@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-24', '2016-10-24'); call addMember(@membershipId,'Chrissy', 'Hadley', 25, null, 'male', null, '', 'clhadley@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="170" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7762,7 +7764,7 @@
       </c>
       <c r="O170" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Kathleen', 'Moore', 25, null, 'male', null, '', 'kmoore@cherrycreekradio.org', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Kathleen', 'Moore', 25, null, 'male', null, '', 'kmoore@cherrycreekradio.org', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="171" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7794,7 +7796,7 @@
       </c>
       <c r="O171" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Michelle', 'Wold', 25, null, 'male', null, '', 'tcmmwold9000@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Michelle', 'Wold', 25, null, 'male', null, '', 'tcmmwold9000@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="172" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7826,7 +7828,7 @@
       </c>
       <c r="O172" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Sarah', 'Storey', 25, null, 'male', null, '', 'sstorey@mtech.edu', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Sarah', 'Storey', 25, null, 'male', null, '', 'sstorey@mtech.edu', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="173" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7858,7 +7860,7 @@
       </c>
       <c r="O173" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Randi', 'Luke', 25, null, 'male', null, '', 'randijo.luke@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Randi', 'Luke', 25, null, 'male', null, '', 'randijo.luke@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="174" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7896,7 +7898,7 @@
       </c>
       <c r="O174" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-03', '2016-10-03'); call addPrimaryMember(@membershipId,'Katherine/James', 'Sweet', 25, null, 'male', null, '', 'kgames1021@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-03', '2016-10-03'); call addMember(@membershipId,'Katherine/James', 'Sweet', 25, null, 'male', null, '', 'kgames1021@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="175" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7928,7 +7930,7 @@
       </c>
       <c r="O175" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Andrew', 'Calderon', 25, null, 'male', null, '', 'tarynj21691@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Andrew', 'Calderon', 25, null, 'male', null, '', 'tarynj21691@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="176" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7963,7 +7965,7 @@
       </c>
       <c r="O176" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-21', '2018-01-21'); call addPrimaryMember(@membershipId,'Ryan/Lindsey', 'Toderovich', 25, null, 'male', null, '', 'lindseytoderovich@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-01-21', '2018-01-21'); call addMember(@membershipId,'Ryan/Lindsey', 'Toderovich', 25, null, 'male', null, '', 'lindseytoderovich@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="177" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -7995,7 +7997,7 @@
       </c>
       <c r="O177" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Logan', 'Dudding', 25, null, 'male', null, '', 'lwdudding@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Logan', 'Dudding', 25, null, 'male', null, '', 'lwdudding@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="178" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8038,7 +8040,7 @@
       </c>
       <c r="O178" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-08', '2018-04-08'); call addPrimaryMember(@membershipId,'Jason/Jennifer', 'Hands', 25, null, 'male', null, '', 'lilyuma@live.com', null, null,'Wiseriver', '59762', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-08', '2018-04-08'); call addMember(@membershipId,'Jason/Jennifer', 'Hands', 25, null, 'male', null, '', 'lilyuma@live.com', null, null,'Wiseriver', '59762', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="179" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8076,7 +8078,7 @@
       </c>
       <c r="O179" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-29', '2018-04-29'); call addPrimaryMember(@membershipId,'Amanda', 'Ortiz-Cabrera', 25, null, 'male', null, '', 'aortiz@mtech.edu', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-29', '2018-04-29'); call addMember(@membershipId,'Amanda', 'Ortiz-Cabrera', 25, null, 'male', null, '', 'aortiz@mtech.edu', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="180" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8096,7 +8098,7 @@
       </c>
       <c r="O180" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'', 'Moran', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'', 'Moran', 25, null, 'male', null, '', '', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="181" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8128,7 +8130,7 @@
       </c>
       <c r="O181" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'James', 'Hadley', 25, null, 'male', null, '', 'mtcarddealer@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'James', 'Hadley', 25, null, 'male', null, '', 'mtcarddealer@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="182" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8163,7 +8165,7 @@
       </c>
       <c r="O182" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-29', '2018-04-29'); call addPrimaryMember(@membershipId,'', 'Persons', 25, null, 'male', null, '', 'twopersons4jesus@bresnan.net', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2017-04-29', '2018-04-29'); call addMember(@membershipId,'', 'Persons', 25, null, 'male', null, '', 'twopersons4jesus@bresnan.net', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="183" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8198,7 +8200,7 @@
       </c>
       <c r="O183" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-24', '2016-10-24'); call addPrimaryMember(@membershipId,'Claudial/Brent', 'Rapkoch', 25, null, 'male', null, '', 'claudiarap59701@msn.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2015-10-24', '2016-10-24'); call addMember(@membershipId,'Claudial/Brent', 'Rapkoch', 25, null, 'male', null, '', 'claudiarap59701@msn.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="184" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8230,7 +8232,7 @@
       </c>
       <c r="O184" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Denise', 'Hendrix', 25, null, 'male', null, '', 'dhendrix49@outlook.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Denise', 'Hendrix', 25, null, 'male', null, '', 'dhendrix49@outlook.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="185" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8262,7 +8264,7 @@
       </c>
       <c r="O185" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Janet/Stephen', 'Coe', 25, null, 'male', null, '', 'janetmcoe@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Janet/Stephen', 'Coe', 25, null, 'male', null, '', 'janetmcoe@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="186" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8294,7 +8296,7 @@
       </c>
       <c r="O186" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Lani', 'Odenbeck', 25, null, 'male', null, '', 'loni.odenbeckdvm@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Lani', 'Odenbeck', 25, null, 'male', null, '', 'loni.odenbeckdvm@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="187" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8326,7 +8328,7 @@
       </c>
       <c r="O187" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Maggie/Logan', 'Matteson', 25, null, 'male', null, '', 'magzrhax@yahoo.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Maggie/Logan', 'Matteson', 25, null, 'male', null, '', 'magzrhax@yahoo.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="188" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8358,7 +8360,7 @@
       </c>
       <c r="O188" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'Lawrence', 'Weirick (Family Outreach)', 25, null, 'male', null, '', 'lawrenw@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'Lawrence', 'Weirick (Family Outreach)', 25, null, 'male', null, '', 'lawrenw@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
     <row r="189" spans="1:15" ht="13" x14ac:dyDescent="0.15">
@@ -8390,7 +8392,7 @@
       </c>
       <c r="O189" t="str">
         <f t="shared" si="8"/>
-        <v>call addMembership('seasonal', 0); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addPrimaryMember(@membershipId,'T', 'McCullak', 25, null, 'male', null, '', 'toshmcc3@gmail.com', null, null,'', '59701', 'MT');</v>
+        <v>call addMembership('seasonal', 0, null); set @membershipId = last_insert_id(); call addMembershipPeriod(@membershipId, '2016-01-01', '2017-01-01'); call addMember(@membershipId,'T', 'McCullak', 25, null, 'male', null, '', 'toshmcc3@gmail.com', null, null,'', '59701', 'MT', @memberId); call updateMembership(@membershipId, 'seasonal', 0, @memberId);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated xls file to generate sql statements with sample data
</commit_message>
<xml_diff>
--- a/SM_testData.xlsx
+++ b/SM_testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coneill/Documents/sm_membership/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F259EE8-925F-374D-A3D8-FB1342CE7813}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93372EF3-0E70-D748-9BB6-9095A671695B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2292,9 +2292,9 @@
   </sheetPr>
   <dimension ref="A1:O189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N124" sqref="N124"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N163" sqref="N163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8667,9 +8667,9 @@
         <f t="shared" si="7"/>
         <v>2017-01-01</v>
       </c>
-      <c r="O186" t="str">
-        <f t="shared" si="8"/>
-        <v>call createMembership('Annual', 0, '2016-01-01', '2017-01-01','Michelle', 'Wold', 25, 'male', 'Unknown'); call addMemberContact((select id from Member where lastName='Wold' and firstName='Michelle'), '', 'tcmmwold9000@gmail.com', null, null,'', '59701', 'MT');</v>
+      <c r="N186" t="str">
+        <f>_xlfn.CONCAT("call addMembershipPeriod((select id from membershipview where primaryMemberFirst='",B186,"' and primaryMemberLast='",A186,"'),'",L186,"','",M186,"');")</f>
+        <v>call addMembershipPeriod((select id from membershipview where primaryMemberFirst='Michelle' and primaryMemberLast='Wold'),'2016-01-01','2017-01-01');</v>
       </c>
     </row>
     <row r="187" spans="1:15" ht="13" x14ac:dyDescent="0.15">

</xml_diff>